<commit_message>
fixe app_comparison_baseline csv table
</commit_message>
<xml_diff>
--- a/app_results/app_comparison_baseline.xlsx
+++ b/app_results/app_comparison_baseline.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Sandisk SSD/app_results/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alexandrawilli/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{582608C3-E438-BC43-B0D9-2684FC3068A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB0A4A10-C9E4-6E4E-AF76-309474350940}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="44060" windowHeight="26900" xr2:uid="{3332F8E0-251F-4B4B-B48E-E2D1080DBF7B}"/>
+    <workbookView xWindow="15940" yWindow="-28340" windowWidth="34400" windowHeight="28340" xr2:uid="{3332F8E0-251F-4B4B-B48E-E2D1080DBF7B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="20">
   <si>
     <t>app name</t>
   </si>
@@ -95,6 +95,9 @@
   </si>
   <si>
     <t>Ensamble</t>
+  </si>
+  <si>
+    <t>Random Forest</t>
   </si>
 </sst>
 </file>
@@ -477,10 +480,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD0FED19-8242-F24A-A3BB-896D7BD1A7B4}">
-  <dimension ref="A1:G37"/>
+  <dimension ref="A1:G46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="303" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="168" workbookViewId="0">
+      <selection activeCell="D51" sqref="D51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -517,10 +520,10 @@
       <c r="C2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="2">
+      <c r="D2" s="1">
         <v>0.95750403442711096</v>
       </c>
-      <c r="E2" s="2">
+      <c r="E2" s="1">
         <v>0.98370798102701495</v>
       </c>
     </row>
@@ -528,17 +531,17 @@
       <c r="A3" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3" s="3">
-        <v>0.1069006781013163</v>
-      </c>
-      <c r="E3" s="3">
-        <v>0.85285118219749645</v>
+      <c r="B3" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="1">
+        <v>0.986966292134831</v>
+      </c>
+      <c r="E3" s="1">
+        <v>0.99758111602302102</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
@@ -546,16 +549,16 @@
         <v>18</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4" s="3">
-        <v>5.6891025641025633E-2</v>
-      </c>
-      <c r="E4" s="3">
-        <v>0.80625424881033303</v>
+        <v>5</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" s="1">
+        <v>0.69968051118210794</v>
+      </c>
+      <c r="E4" s="1">
+        <v>0.978336022124913</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
@@ -563,16 +566,16 @@
         <v>18</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D5">
-        <v>0.97524314765693998</v>
-      </c>
-      <c r="E5">
-        <v>0.99531459170013303</v>
+        <v>6</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" s="1">
+        <v>0.76698014629049105</v>
+      </c>
+      <c r="E5" s="1">
+        <v>0.972479328643712</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
@@ -580,16 +583,16 @@
         <v>18</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D6" s="2">
-        <v>0.986966292134831</v>
-      </c>
-      <c r="E6" s="2">
-        <v>0.99758111602302102</v>
+      <c r="D6" s="1">
+        <v>0.87099841521394605</v>
+      </c>
+      <c r="E6" s="1">
+        <v>0.93107535986452095</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
@@ -597,16 +600,16 @@
         <v>18</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D7" s="3">
-        <v>0.95006839945280397</v>
-      </c>
-      <c r="E7" s="3">
-        <v>0.9902310853601024</v>
+        <v>11</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D7" s="1">
+        <v>0.72043852779952999</v>
+      </c>
+      <c r="E7" s="1">
+        <v>0.72906653174803904</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
@@ -614,16 +617,16 @@
         <v>18</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D8" s="3">
-        <v>0.76360637713029134</v>
-      </c>
-      <c r="E8" s="3">
-        <v>5.6283231746855143E-2</v>
+        <v>8</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D8" s="1">
+        <v>0.77544910179640703</v>
+      </c>
+      <c r="E8" s="1">
+        <v>0.95992519369489704</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
@@ -631,33 +634,33 @@
         <v>18</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C9" t="s">
-        <v>16</v>
-      </c>
-      <c r="D9">
-        <v>0.96034763715372096</v>
-      </c>
-      <c r="E9">
-        <v>0.98500102732689498</v>
+        <v>7</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D9" s="1">
+        <v>0.95464362850971896</v>
+      </c>
+      <c r="E9" s="1">
+        <v>0.967914438502673</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="2" t="s">
-        <v>5</v>
+      <c r="B10" s="4" t="s">
+        <v>9</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D10" s="2">
-        <v>0.69968051118210794</v>
-      </c>
-      <c r="E10" s="2">
-        <v>0.978336022124913</v>
+      <c r="D10" s="1">
+        <v>2.6666666666666599E-2</v>
+      </c>
+      <c r="E10" s="1">
+        <v>0.94011484823625902</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
@@ -665,33 +668,33 @@
         <v>18</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D11" s="3">
-        <v>0.4416015162283819</v>
+        <v>0.1069006781013163</v>
       </c>
       <c r="E11" s="3">
-        <v>0.93041610470053449</v>
+        <v>0.85285118219749645</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>18</v>
       </c>
-      <c r="B12" s="2" t="s">
-        <v>5</v>
+      <c r="B12" s="4" t="s">
+        <v>2</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D12" s="3">
-        <v>0.45664739884393102</v>
+        <v>0.95006839945280397</v>
       </c>
       <c r="E12" s="3">
-        <v>0.79583057577763083</v>
+        <v>0.9902310853601024</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
@@ -701,14 +704,14 @@
       <c r="B13" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C13" t="s">
-        <v>16</v>
-      </c>
-      <c r="D13">
-        <v>0.69717772692600999</v>
-      </c>
-      <c r="E13">
-        <v>0.94876758291392405</v>
+      <c r="C13" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D13" s="3">
+        <v>0.4416015162283819</v>
+      </c>
+      <c r="E13" s="3">
+        <v>0.93041610470053449</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
@@ -718,31 +721,31 @@
       <c r="B14" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C14" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D14" s="2">
-        <v>0.76698014629049105</v>
-      </c>
-      <c r="E14" s="2">
-        <v>0.972479328643712</v>
+      <c r="C14" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D14" s="3">
+        <v>0.56034051076614921</v>
+      </c>
+      <c r="E14" s="3">
+        <v>0.91437081161578548</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>18</v>
       </c>
-      <c r="B15" s="2" t="s">
-        <v>6</v>
+      <c r="B15" s="4" t="s">
+        <v>10</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D15" s="3">
-        <v>0.56034051076614921</v>
+        <v>0.65556915544675598</v>
       </c>
       <c r="E15" s="3">
-        <v>0.91437081161578548</v>
+        <v>0.63720546438067294</v>
       </c>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
@@ -751,17 +754,17 @@
       <c r="A16" t="s">
         <v>18</v>
       </c>
-      <c r="B16" s="2" t="s">
-        <v>6</v>
+      <c r="B16" s="4" t="s">
+        <v>11</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D16" s="3">
-        <v>0.441159077468953</v>
+        <v>0.34102952308856932</v>
       </c>
       <c r="E16" s="3">
-        <v>0.7244891582828219</v>
+        <v>0.7518711241000785</v>
       </c>
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
@@ -770,17 +773,17 @@
       <c r="A17" t="s">
         <v>18</v>
       </c>
-      <c r="B17" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C17" t="s">
-        <v>16</v>
-      </c>
-      <c r="D17">
-        <v>0.53471502590673503</v>
-      </c>
-      <c r="E17">
-        <v>0.94615661350281799</v>
+      <c r="B17" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D17" s="8">
+        <v>0.64096916299999995</v>
+      </c>
+      <c r="E17" s="5">
+        <v>0.90583471199999999</v>
       </c>
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
@@ -790,16 +793,16 @@
         <v>18</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D18" s="2">
-        <v>0.87099841521394605</v>
-      </c>
-      <c r="E18" s="2">
-        <v>0.93107535986452095</v>
+        <v>7</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D18" s="3">
+        <v>5.1162790697674432E-2</v>
+      </c>
+      <c r="E18" s="3">
+        <v>0.75590368436321442</v>
       </c>
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
@@ -809,16 +812,16 @@
         <v>18</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C19" s="3" t="s">
         <v>14</v>
       </c>
       <c r="D19" s="3">
-        <v>0.65556915544675598</v>
+        <v>0.37368050668543301</v>
       </c>
       <c r="E19" s="3">
-        <v>0.63720546438067294</v>
+        <v>0.74052478134110788</v>
       </c>
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
@@ -827,17 +830,17 @@
       <c r="A20" t="s">
         <v>18</v>
       </c>
-      <c r="B20" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D20" s="3">
-        <v>0.60176458792861443</v>
-      </c>
-      <c r="E20" s="3">
-        <v>0.6859262767384956</v>
+      <c r="B20" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C20" t="s">
+        <v>16</v>
+      </c>
+      <c r="D20">
+        <v>0.96034763715372096</v>
+      </c>
+      <c r="E20">
+        <v>0.98500102732689498</v>
       </c>
       <c r="F20" s="1"/>
       <c r="G20" s="1"/>
@@ -847,16 +850,16 @@
         <v>18</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="C21" t="s">
         <v>16</v>
       </c>
       <c r="D21">
-        <v>0.73817034700315398</v>
+        <v>0.97524314765693998</v>
       </c>
       <c r="E21">
-        <v>0.94265579660080101</v>
+        <v>0.99531459170013303</v>
       </c>
       <c r="F21" s="1"/>
       <c r="G21" s="1"/>
@@ -865,34 +868,34 @@
       <c r="A22" t="s">
         <v>18</v>
       </c>
-      <c r="B22" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D22" s="2">
-        <v>0.72043852779952999</v>
-      </c>
-      <c r="E22" s="2">
-        <v>0.72906653174803904</v>
+      <c r="B22" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C22" t="s">
+        <v>16</v>
+      </c>
+      <c r="D22">
+        <v>0.53471502590673503</v>
+      </c>
+      <c r="E22">
+        <v>0.94615661350281799</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>18</v>
       </c>
-      <c r="B23" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D23" s="3">
-        <v>0.34102952308856932</v>
-      </c>
-      <c r="E23" s="3">
-        <v>0.7518711241000785</v>
+      <c r="B23" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C23" t="s">
+        <v>16</v>
+      </c>
+      <c r="D23">
+        <v>0.69717772692600999</v>
+      </c>
+      <c r="E23">
+        <v>0.94876758291392405</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
@@ -900,16 +903,16 @@
         <v>18</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C24" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D24" s="3">
-        <v>0.3274177467597208</v>
-      </c>
-      <c r="E24" s="3">
-        <v>0.69808356896010049</v>
+        <v>10</v>
+      </c>
+      <c r="C24" t="s">
+        <v>16</v>
+      </c>
+      <c r="D24">
+        <v>0.731212540341171</v>
+      </c>
+      <c r="E24">
+        <v>0.75307073274036396</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
@@ -923,10 +926,10 @@
         <v>16</v>
       </c>
       <c r="D25">
-        <v>0.53300124533001203</v>
+        <v>0.72453371592539395</v>
       </c>
       <c r="E25">
-        <v>0.87820721013316005</v>
+        <v>0.68017767906718396</v>
       </c>
     </row>
     <row r="26" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -936,14 +939,14 @@
       <c r="B26" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C26" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D26" s="2">
-        <v>0.77544910179640703</v>
-      </c>
-      <c r="E26" s="2">
-        <v>0.95992519369489704</v>
+      <c r="C26" t="s">
+        <v>16</v>
+      </c>
+      <c r="D26">
+        <v>0.73817034700315398</v>
+      </c>
+      <c r="E26">
+        <v>0.94265579660080101</v>
       </c>
       <c r="F26" s="2"/>
     </row>
@@ -952,50 +955,50 @@
         <v>18</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C27" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D27" s="8">
-        <v>0.64096916299999995</v>
-      </c>
-      <c r="E27" s="5">
-        <v>0.90583471199999999</v>
+        <v>7</v>
+      </c>
+      <c r="C27" t="s">
+        <v>16</v>
+      </c>
+      <c r="D27">
+        <v>0.838741156379604</v>
+      </c>
+      <c r="E27">
+        <v>0.86345796323073698</v>
       </c>
     </row>
     <row r="28" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>18</v>
       </c>
-      <c r="B28" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D28" s="2">
-        <v>0.255517759670912</v>
-      </c>
-      <c r="E28" s="2">
-        <v>0.64740610799999998</v>
+      <c r="B28" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C28" t="s">
+        <v>16</v>
+      </c>
+      <c r="D28">
+        <v>0.53300124533001203</v>
+      </c>
+      <c r="E28">
+        <v>0.87820721013316005</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>18</v>
       </c>
-      <c r="B29" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C29" t="s">
-        <v>16</v>
-      </c>
-      <c r="D29">
-        <v>0.838741156379604</v>
-      </c>
-      <c r="E29">
-        <v>0.86345796323073698</v>
+      <c r="B29" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D29" s="1">
+        <v>0.96077377753895699</v>
+      </c>
+      <c r="E29" s="1">
+        <v>0.98493913761089302</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
@@ -1003,50 +1006,50 @@
         <v>18</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D30" s="2">
-        <v>0.95464362850971896</v>
-      </c>
-      <c r="E30" s="2">
-        <v>0.967914438502673</v>
+        <v>2</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D30" s="1">
+        <v>0.98746642793196004</v>
+      </c>
+      <c r="E30" s="1">
+        <v>0.99766277128547498</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>18</v>
       </c>
-      <c r="B31" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C31" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D31" s="3">
-        <v>5.1162790697674432E-2</v>
-      </c>
-      <c r="E31" s="3">
-        <v>0.75590368436321442</v>
+      <c r="B31" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D31" s="1">
+        <v>0.67333333333333301</v>
+      </c>
+      <c r="E31" s="1">
+        <v>0.97748161764705799</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>18</v>
       </c>
-      <c r="B32" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C32" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D32" s="3">
-        <v>0.47148288973384028</v>
-      </c>
-      <c r="E32" s="3">
-        <v>0.76497569658383002</v>
+      <c r="B32" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D32" s="1">
+        <v>0.77262693156732798</v>
+      </c>
+      <c r="E32" s="1">
+        <v>0.97473632572970303</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
@@ -1054,16 +1057,16 @@
         <v>18</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C33" t="s">
-        <v>16</v>
-      </c>
-      <c r="D33">
-        <v>0.731212540341171</v>
-      </c>
-      <c r="E33">
-        <v>0.75307073274036396</v>
+        <v>10</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D33" s="1">
+        <v>0.857053094564875</v>
+      </c>
+      <c r="E33" s="1">
+        <v>0.92257954738812298</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
@@ -1071,73 +1074,226 @@
         <v>18</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C34" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D34" s="2">
-        <v>2.6666666666666599E-2</v>
-      </c>
-      <c r="E34" s="2">
-        <v>0.94011484823625902</v>
+        <v>11</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D34" s="1">
+        <v>0.72203120867495296</v>
+      </c>
+      <c r="E34" s="1">
+        <v>0.73744691481388902</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>18</v>
       </c>
-      <c r="B35" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C35" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D35" s="3">
-        <v>0.37368050668543301</v>
-      </c>
-      <c r="E35" s="3">
-        <v>0.74052478134110788</v>
+      <c r="B35" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D35" s="1">
+        <v>0.77166541070082895</v>
+      </c>
+      <c r="E35" s="1">
+        <v>0.95957304869913196</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>18</v>
       </c>
-      <c r="B36" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C36" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D36" s="2">
-        <v>0.21789084940500619</v>
-      </c>
-      <c r="E36" s="2">
-        <v>0.64740610799999998</v>
+      <c r="B36" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D36" s="1">
+        <v>0.95905172413793105</v>
+      </c>
+      <c r="E36" s="1">
+        <v>0.97092578423871401</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>18</v>
       </c>
-      <c r="B37" s="4" t="s">
+      <c r="B37" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C37" t="s">
-        <v>16</v>
-      </c>
-      <c r="D37">
-        <v>0.72453371592539395</v>
-      </c>
-      <c r="E37">
-        <v>0.68017767906718396</v>
+      <c r="C37" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D37" s="1">
+        <v>1.8348623853211E-2</v>
+      </c>
+      <c r="E37" s="1">
+        <v>0.941593886462882</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>18</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D38" s="3">
+        <v>5.6891025641025633E-2</v>
+      </c>
+      <c r="E38" s="3">
+        <v>0.80625424881033303</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>18</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D39" s="3">
+        <v>0.76360637713029134</v>
+      </c>
+      <c r="E39" s="3">
+        <v>5.6283231746855143E-2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>18</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D40" s="3">
+        <v>0.45664739884393102</v>
+      </c>
+      <c r="E40" s="3">
+        <v>0.79583057577763083</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>18</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D41" s="3">
+        <v>0.441159077468953</v>
+      </c>
+      <c r="E41" s="3">
+        <v>0.7244891582828219</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>18</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D42" s="3">
+        <v>0.60176458792861443</v>
+      </c>
+      <c r="E42" s="3">
+        <v>0.6859262767384956</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>18</v>
+      </c>
+      <c r="B43" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D43" s="3">
+        <v>0.3274177467597208</v>
+      </c>
+      <c r="E43" s="3">
+        <v>0.69808356896010049</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>18</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D44" s="2">
+        <v>0.255517759670912</v>
+      </c>
+      <c r="E44" s="2">
+        <v>0.64740610799999998</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>18</v>
+      </c>
+      <c r="B45" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D45" s="3">
+        <v>0.47148288973384028</v>
+      </c>
+      <c r="E45" s="3">
+        <v>0.76497569658383002</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>18</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D46" s="2">
+        <v>0.21789084940500619</v>
+      </c>
+      <c r="E46" s="2">
+        <v>0.64740610799999998</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="B1:E28" xr:uid="{DD0FED19-8242-F24A-A3BB-896D7BD1A7B4}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:E37">
-      <sortCondition ref="B1:B37"/>
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:E46">
+      <sortCondition ref="C1:C46"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>